<commit_message>
update xlsx template to current version
</commit_message>
<xml_diff>
--- a/traitdata_template.xlsx
+++ b/traitdata_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="17715" windowHeight="7485" tabRatio="700" activeTab="6"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="17715" windowHeight="7485" tabRatio="700"/>
   </bookViews>
   <sheets>
     <sheet name="Traitdata_original" sheetId="6" r:id="rId1"/>
@@ -21,17 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>occurenceID</t>
   </si>
   <si>
-    <t>occurenceID_original</t>
-  </si>
-  <si>
-    <t>scientificName_original</t>
-  </si>
-  <si>
     <t>scientificName</t>
   </si>
   <si>
@@ -44,30 +38,9 @@
     <t>kingdom</t>
   </si>
   <si>
-    <t>measurementType_original</t>
-  </si>
-  <si>
-    <t>measurementType</t>
-  </si>
-  <si>
-    <t>measurementValue_original</t>
-  </si>
-  <si>
-    <t>measurementUnit_original</t>
-  </si>
-  <si>
-    <t>measurementValue</t>
-  </si>
-  <si>
-    <t>measurementUnit</t>
-  </si>
-  <si>
     <t>measurementID</t>
   </si>
   <si>
-    <t>measurementID_original</t>
-  </si>
-  <si>
     <t>warnings</t>
   </si>
   <si>
@@ -212,9 +185,6 @@
     <t>MinAllowedValue</t>
   </si>
   <si>
-    <t>MeasurementTypeDescription</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -239,14 +209,44 @@
     <t>ValueType</t>
   </si>
   <si>
-    <t>measurementTypeID</t>
+    <t>traitName</t>
+  </si>
+  <si>
+    <t>traitValue</t>
+  </si>
+  <si>
+    <t>traitUnit</t>
+  </si>
+  <si>
+    <t>traitID</t>
+  </si>
+  <si>
+    <t>scientificNameStd</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>traitNameStd</t>
+  </si>
+  <si>
+    <t>traitValueStd</t>
+  </si>
+  <si>
+    <t>traitUnitStd</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>traitDescription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -724,8 +731,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1073,13 +1081,14 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="27.140625" customWidth="1"/>
+    <col min="1" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,23 +1096,24 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1112,47 +1122,44 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1167,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,49 +1199,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1256,9 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1282,67 +1291,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
         <v>41</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1368,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,16 +1384,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1410,27 +1419,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1440,32 +1449,38 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1477,9 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1492,49 +1505,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>